<commit_message>
Add rotor temp sensor definition
</commit_message>
<xml_diff>
--- a/design/SensorUnit_2023-05-28.xlsx
+++ b/design/SensorUnit_2023-05-28.xlsx
@@ -1,41 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\HavirNAS\Documents\Tomek\pojazdy\Miata30\KnurDash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\KnurDash\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8230D799-476D-489F-9412-E78AC20E1C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3A662F-CCD0-4CE5-9B63-876782EF8460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{C15B9210-5287-4BB4-843A-B886E7D7C4FA}"/>
+    <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{C15B9210-5287-4BB4-843A-B886E7D7C4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcs" sheetId="1" r:id="rId1"/>
-    <sheet name="pinouts" sheetId="4" r:id="rId2"/>
-    <sheet name="temp" sheetId="3" r:id="rId3"/>
-    <sheet name="pressure" sheetId="2" r:id="rId4"/>
+    <sheet name="Pinouts" sheetId="4" r:id="rId2"/>
+    <sheet name="Temp" sheetId="3" r:id="rId3"/>
+    <sheet name="Pressure" sheetId="2" r:id="rId4"/>
+    <sheet name="RotorTemp" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="polA">temp!$E$2</definedName>
-    <definedName name="polA2">temp!#REF!</definedName>
-    <definedName name="polB">temp!$F$2</definedName>
-    <definedName name="polB2">temp!#REF!</definedName>
-    <definedName name="polC">temp!$G$2</definedName>
-    <definedName name="polC2">temp!#REF!</definedName>
-    <definedName name="polD">temp!#REF!</definedName>
-    <definedName name="polE">temp!#REF!</definedName>
-    <definedName name="ppolA">pressure!$G$2</definedName>
-    <definedName name="ppolB">pressure!$H$2</definedName>
-    <definedName name="ppolC">pressure!$I$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">pinouts!$A$1:$AH$38</definedName>
-    <definedName name="PsiToBar">pressure!$B$2</definedName>
+    <definedName name="polA">Temp!$E$2</definedName>
+    <definedName name="polA2">Temp!#REF!</definedName>
+    <definedName name="polB">Temp!$F$2</definedName>
+    <definedName name="polB2">Temp!#REF!</definedName>
+    <definedName name="polC">Temp!$G$2</definedName>
+    <definedName name="polC2">Temp!#REF!</definedName>
+    <definedName name="polD">Temp!#REF!</definedName>
+    <definedName name="polE">Temp!#REF!</definedName>
+    <definedName name="ppolA">Pressure!$G$2</definedName>
+    <definedName name="ppolB">Pressure!$H$2</definedName>
+    <definedName name="ppolC">Pressure!$I$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Pinouts!$A$1:$AH$38</definedName>
+    <definedName name="PsiToBar">Pressure!$B$2</definedName>
+    <definedName name="ROTOR_A">RotorTemp!$C$14</definedName>
+    <definedName name="ROTOR_B">RotorTemp!$C$15</definedName>
     <definedName name="Rref">Calcs!$C$13</definedName>
     <definedName name="Rsensor">Calcs!$C$14</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">pressure!$G$2:$I$2</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">temp!$E$2:$G$2</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Pressure!$G$2:$I$2</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Temp!$E$2:$G$2</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
@@ -62,8 +65,8 @@
     <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">pressure!$M$36</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">temp!$H$50</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Pressure!$M$36</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Temp!$H$50</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
@@ -101,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="149">
   <si>
     <t>Vin</t>
   </si>
@@ -533,6 +536,21 @@
   </si>
   <si>
     <t>RESET BTN</t>
+  </si>
+  <si>
+    <t>V+</t>
+  </si>
+  <si>
+    <t>V-min</t>
+  </si>
+  <si>
+    <t>V-max</t>
+  </si>
+  <si>
+    <t>VtotalMin</t>
+  </si>
+  <si>
+    <t>VtotalMax</t>
   </si>
 </sst>
 </file>
@@ -954,7 +972,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>temp!$B$4:$B$48</c:f>
+              <c:f>Temp!$B$4:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
@@ -1098,7 +1116,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>temp!$E$4:$E$48</c:f>
+              <c:f>Temp!$E$4:$E$48</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="45"/>
@@ -1276,7 +1294,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>temp!$B$8:$B$49</c:f>
+              <c:f>Temp!$B$8:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="42"/>
@@ -1408,7 +1426,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>temp!$C$8:$C$45</c:f>
+              <c:f>Temp!$C$8:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="38"/>
@@ -1775,7 +1793,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>pressure!$B$5:$B$34</c:f>
+              <c:f>Pressure!$B$5:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1874,7 +1892,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>pressure!$E$5:$E$34</c:f>
+              <c:f>Pressure!$E$5:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2007,7 +2025,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>pressure!$B$5:$B$33</c:f>
+              <c:f>Pressure!$B$5:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="29"/>
@@ -2103,7 +2121,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>pressure!$C$5:$C$33</c:f>
+              <c:f>Pressure!$C$5:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="29"/>
@@ -2393,6 +2411,443 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="34925" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>RotorTemp!$G$2:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>RotorTemp!$H$2:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>187.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>312.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>437.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>562.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>687.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>812.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>937.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3E46-46D3-A1F2-9C5DC5CD96D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="900711248"/>
+        <c:axId val="827917824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="900711248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="827917824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="827917824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900711248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2434,6 +2889,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3505,6 +4000,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3863,6 +4874,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>16979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>110987</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68332</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28EBBF35-5924-59C3-BD27-620160760155}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4163,7 +5215,7 @@
   <dimension ref="B2:S36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4654,7 +5706,7 @@
   </sheetPr>
   <dimension ref="B1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -6703,8 +7755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B5F49D-8C3A-42CF-AA09-87F9A0902ABA}">
   <dimension ref="B1:M64"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7846,4 +8898,243 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66658717-C5D7-4239-91FE-70F1BC01BC7C}">
+  <dimension ref="B1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7">
+        <f>(C3/1000)*C5</f>
+        <v>0.188</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>312.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8">
+        <f>(C4/1000)*C5</f>
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9">
+        <f>C2-C8</f>
+        <v>11.06</v>
+      </c>
+      <c r="G9">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>437.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10">
+        <f>C2-C7</f>
+        <v>11.811999999999999</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <v>562.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>687.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>-250</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>62.5</v>
+      </c>
+      <c r="G15">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>812.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>18</v>
+      </c>
+      <c r="H16">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>19</v>
+      </c>
+      <c r="H17">
+        <v>937.5</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>20</v>
+      </c>
+      <c r="H18">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to sensor calcs
</commit_message>
<xml_diff>
--- a/design/SensorUnit_2023-05-28.xlsx
+++ b/design/SensorUnit_2023-05-28.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\KnurDash\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3A662F-CCD0-4CE5-9B63-876782EF8460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E44054E-46AF-4AC1-A292-AC171036AA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{C15B9210-5287-4BB4-843A-B886E7D7C4FA}"/>
   </bookViews>
@@ -8905,7 +8905,7 @@
   <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updates to SensorUnit; design for trans pump
</commit_message>
<xml_diff>
--- a/design/SensorUnit_2023-05-28.xlsx
+++ b/design/SensorUnit_2023-05-28.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\KnurDash\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B185B52D-7C54-4623-87AA-28147D7197CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55071A79-073F-4331-AF0C-9BD20E3F4F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" xr2:uid="{C15B9210-5287-4BB4-843A-B886E7D7C4FA}"/>
+    <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{C15B9210-5287-4BB4-843A-B886E7D7C4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcs" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="169">
   <si>
     <t>Vin</t>
   </si>
@@ -297,9 +297,6 @@
     <t>BLU</t>
   </si>
   <si>
-    <t>GRY</t>
-  </si>
-  <si>
     <t>BRO</t>
   </si>
   <si>
@@ -307,18 +304,6 @@
   </si>
   <si>
     <t>YLL</t>
-  </si>
-  <si>
-    <t>SU I2C0 DATA</t>
-  </si>
-  <si>
-    <t>SU I2C0 CLK</t>
-  </si>
-  <si>
-    <t>SU UART_TX</t>
-  </si>
-  <si>
-    <t>SU UART_RX</t>
   </si>
   <si>
     <t>SU GND</t>
@@ -444,9 +429,6 @@
     <t>Oil Temp</t>
   </si>
   <si>
-    <t>Channel</t>
-  </si>
-  <si>
     <t>Oil Press</t>
   </si>
   <si>
@@ -555,9 +537,6 @@
     <t>VtotalMax</t>
   </si>
   <si>
-    <t>RotorTemp</t>
-  </si>
-  <si>
     <t>1x1</t>
   </si>
   <si>
@@ -628,6 +607,42 @@
   </si>
   <si>
     <t>v-max</t>
+  </si>
+  <si>
+    <t>sensor connector 2</t>
+  </si>
+  <si>
+    <t>caliper temp</t>
+  </si>
+  <si>
+    <t>1x2</t>
+  </si>
+  <si>
+    <t>sensor connector 1</t>
+  </si>
+  <si>
+    <t>RotorTemp 1</t>
+  </si>
+  <si>
+    <t>RotorTemp Power</t>
+  </si>
+  <si>
+    <t>ADC Channel</t>
+  </si>
+  <si>
+    <t>TRANS PUMP</t>
+  </si>
+  <si>
+    <t>trans pump</t>
+  </si>
+  <si>
+    <t>ground</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>5V to on</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1000,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1018,6 +1032,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -8587,7 +8604,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>48283</xdr:colOff>
+      <xdr:colOff>48284</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>199003</xdr:rowOff>
     </xdr:to>
@@ -9224,7 +9241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3140C9DF-2692-47E8-B5FD-96C592C7023B}">
   <dimension ref="B2:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -9260,7 +9277,7 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="34"/>
+      <c r="S4" s="33"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -9272,7 +9289,7 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="34"/>
+      <c r="S5" s="33"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -9342,7 +9359,7 @@
         <v>20.333929636255217</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E15">
         <f>Vout*2</f>
@@ -9356,45 +9373,45 @@
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G20" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H20" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="I20" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="J20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="K20" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="M20" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="N20" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>2000</v>
@@ -9429,7 +9446,7 @@
         <f t="shared" si="2"/>
         <v>1833.3333333333335</v>
       </c>
-      <c r="L21" s="34">
+      <c r="L21" s="33">
         <f>Vin*G21/1000</f>
         <v>2.4199999999999998E-3</v>
       </c>
@@ -9452,7 +9469,7 @@
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C22">
         <v>465</v>
@@ -9487,7 +9504,7 @@
         <f t="shared" si="2"/>
         <v>992.48120300751884</v>
       </c>
-      <c r="L22" s="34">
+      <c r="L22" s="33">
         <f>Vin*G22/1000</f>
         <v>1.6375939849624061E-2</v>
       </c>
@@ -9518,7 +9535,7 @@
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C23">
         <v>20000</v>
@@ -9553,7 +9570,7 @@
         <f t="shared" si="2"/>
         <v>2030.7692307692307</v>
       </c>
-      <c r="L23" s="34">
+      <c r="L23" s="33">
         <f>Vin*G23/1000</f>
         <v>2.0942307692307691E-4</v>
       </c>
@@ -9576,49 +9593,49 @@
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C25">
         <v>162</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="38">
+        <v>81</v>
+      </c>
+      <c r="C26" s="37">
         <f>Vin*1000-C25</f>
         <v>3138</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F26" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G26" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I26" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J26" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="K26" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="L26" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
@@ -9648,7 +9665,7 @@
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="38">
+      <c r="C28" s="37">
         <f>C26/C27</f>
         <v>1.569</v>
       </c>
@@ -9671,7 +9688,7 @@
         <f>I27</f>
         <v>3.31</v>
       </c>
-      <c r="J28" s="37">
+      <c r="J28" s="36">
         <f>-F28*G28*LN(I28/H28)</f>
         <v>-7.1104441538622117E-4</v>
       </c>
@@ -9688,7 +9705,7 @@
       <c r="B29" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="39">
+      <c r="C29" s="38">
         <f>C25/C28</f>
         <v>103.25047801147228</v>
       </c>
@@ -9698,21 +9715,21 @@
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="40">
+        <v>83</v>
+      </c>
+      <c r="C30" s="39">
         <f>polA+polB*LN(C29)+polC*(LN(C29))^3</f>
         <v>100.14530084854968</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="40">
+        <v>126</v>
+      </c>
+      <c r="C31" s="39">
         <f>ppolA+ppolB*C29+ppolC*C29^2</f>
         <v>2.6878289098074597</v>
       </c>
@@ -9722,18 +9739,18 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -9771,17 +9788,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AFCC8DD-5DD0-4266-935E-E84E0B0CCB9F}">
   <dimension ref="B1:Q34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
     <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="5.140625" customWidth="1"/>
@@ -9792,7 +9810,7 @@
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
@@ -9813,14 +9831,14 @@
         <v>2</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="44" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="9">
@@ -9854,7 +9872,7 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="43" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="9">
@@ -9868,7 +9886,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O4" s="17" t="s">
         <v>46</v>
@@ -9878,7 +9896,7 @@
         <v>6</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -9888,14 +9906,14 @@
       <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="45" t="s">
         <v>32</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
@@ -9904,35 +9922,30 @@
       <c r="N5" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="23" t="s">
-        <v>53</v>
-      </c>
+      <c r="O5" s="11"/>
       <c r="P5">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="Q5" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F6" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="24" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
@@ -9941,16 +9954,11 @@
       <c r="N6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="24" t="s">
-        <v>54</v>
-      </c>
+      <c r="O6" s="11"/>
       <c r="P6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="Q6" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -9962,21 +9970,21 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="46" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="9">
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7">
@@ -9994,21 +10002,21 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="47" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="9">
         <v>5</v>
       </c>
       <c r="L8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="N8" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O8" s="17" t="s">
         <v>46</v>
@@ -10018,40 +10026,45 @@
         <v>14</v>
       </c>
       <c r="Q8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F9" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" s="50" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="9">
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="O9" s="11"/>
+        <v>54</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="P9">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
+      <c r="Q9" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>148</v>
-      </c>
-      <c r="F10" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="49" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="9">
@@ -10070,13 +10083,13 @@
     </row>
     <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F11" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="51" t="s">
         <v>39</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
@@ -10091,13 +10104,13 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>146</v>
-      </c>
-      <c r="F12" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="52" t="s">
         <v>38</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
@@ -10135,9 +10148,6 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="L15" t="s">
-        <v>57</v>
-      </c>
       <c r="M15">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -10148,11 +10158,11 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="Q15" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H16" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="M16">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -10166,16 +10176,16 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
@@ -10189,20 +10199,20 @@
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="26" t="s">
-        <v>77</v>
+      <c r="B18" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="M18">
         <f t="shared" si="0"/>
@@ -10216,20 +10226,20 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="28" t="s">
-        <v>79</v>
+        <v>101</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>74</v>
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
@@ -10243,19 +10253,19 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
-        <v>76</v>
+      <c r="B20" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="24" t="s">
         <v>33</v>
       </c>
       <c r="M20">
@@ -10270,20 +10280,20 @@
       </c>
     </row>
     <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="28" t="s">
-        <v>79</v>
+      <c r="B21" s="27" t="s">
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>83</v>
+        <v>99</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>78</v>
       </c>
       <c r="M21">
         <f t="shared" si="0"/>
@@ -10297,76 +10307,126 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
-        <v>81</v>
+      <c r="B22" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
-        <v>83</v>
+      <c r="B23" s="29" t="s">
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="G23" t="s">
-        <v>140</v>
-      </c>
-      <c r="H23" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="I23" s="43" t="s">
-        <v>143</v>
+        <v>133</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>162</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G25" t="s">
-        <v>142</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="G30" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>35</v>
+      </c>
       <c r="G31" s="9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" t="s">
+        <v>168</v>
+      </c>
       <c r="G32" s="9" t="s">
         <v>41</v>
       </c>
       <c r="H32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="9"/>
+      <c r="D33" s="25" t="s">
+        <v>71</v>
+      </c>
       <c r="G33" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>30</v>
+      </c>
       <c r="G34" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H34" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -10413,7 +10473,7 @@
       <c r="F2" s="2">
         <v>-39.954820138689989</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="31">
         <v>9.1362491468999538E-2</v>
       </c>
     </row>
@@ -10560,15 +10620,15 @@
       <c r="C8" s="3">
         <v>91.111111111111114</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <f>polA+polB*LN(B8)+polC*(LN(B8))^3</f>
         <v>89.894649327124952</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <f t="shared" si="3"/>
         <v>1.200000000000004</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="32">
         <f t="shared" si="1"/>
         <v>91.094649327124955</v>
       </c>
@@ -10588,15 +10648,15 @@
       <c r="C9" s="3">
         <v>87.777777777777771</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <f t="shared" si="0"/>
         <v>87.168485482688169</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <f t="shared" si="3"/>
         <v>1.2150000000000039</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="32">
         <f t="shared" si="1"/>
         <v>88.383485482688172</v>
       </c>
@@ -10616,15 +10676,15 @@
       <c r="C10" s="3">
         <v>85.555555555555557</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="32">
         <f t="shared" si="0"/>
         <v>84.466627703579547</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <f t="shared" si="3"/>
         <v>1.2300000000000038</v>
       </c>
-      <c r="G10" s="33">
+      <c r="G10" s="32">
         <f t="shared" si="1"/>
         <v>85.696627703579551</v>
       </c>
@@ -10644,15 +10704,15 @@
       <c r="C11" s="3">
         <v>83.333333333333329</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="32">
         <f t="shared" si="0"/>
         <v>81.622511925461069</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="32">
         <f t="shared" si="3"/>
         <v>1.2450000000000037</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="32">
         <f t="shared" si="1"/>
         <v>82.867511925461073</v>
       </c>
@@ -10672,15 +10732,15 @@
       <c r="C12" s="3">
         <v>81.111111111111114</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="32">
         <f t="shared" si="0"/>
         <v>79.02520244509617</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <f t="shared" si="3"/>
         <v>1.2600000000000036</v>
       </c>
-      <c r="G12" s="33">
+      <c r="G12" s="32">
         <f t="shared" si="1"/>
         <v>80.285202445096175</v>
       </c>
@@ -10700,15 +10760,15 @@
       <c r="C13" s="3">
         <v>78.888888888888886</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <f t="shared" si="0"/>
         <v>77.411794184060966</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <f t="shared" si="3"/>
         <v>1.2750000000000035</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="32">
         <f t="shared" si="1"/>
         <v>78.686794184060972</v>
       </c>
@@ -10728,15 +10788,15 @@
       <c r="C14" s="3">
         <v>76.666666666666671</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="32">
         <f t="shared" si="0"/>
         <v>75.733340023153175</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <f t="shared" si="3"/>
         <v>1.2900000000000034</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="32">
         <f t="shared" si="1"/>
         <v>77.023340023153182</v>
       </c>
@@ -10756,15 +10816,15 @@
       <c r="C15" s="3">
         <v>75.555555555555557</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="32">
         <f t="shared" si="0"/>
         <v>74.286551151136905</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="32">
         <f t="shared" si="3"/>
         <v>1.3050000000000033</v>
       </c>
-      <c r="G15" s="33">
+      <c r="G15" s="32">
         <f t="shared" si="1"/>
         <v>75.591551151136912</v>
       </c>
@@ -10784,15 +10844,15 @@
       <c r="C16" s="3">
         <v>75</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="32">
         <f t="shared" si="0"/>
         <v>73.727318675192208</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="32">
         <f t="shared" si="3"/>
         <v>1.3200000000000032</v>
       </c>
-      <c r="G16" s="33">
+      <c r="G16" s="32">
         <f t="shared" si="1"/>
         <v>75.047318675192216</v>
       </c>
@@ -10812,15 +10872,15 @@
       <c r="C17" s="3">
         <v>73.333333333333329</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="32">
         <f t="shared" si="0"/>
         <v>72.507008164972135</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="32">
         <f t="shared" si="3"/>
         <v>1.3350000000000031</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="32">
         <f t="shared" si="1"/>
         <v>73.842008164972142</v>
       </c>
@@ -10840,15 +10900,15 @@
       <c r="C18" s="3">
         <v>72.222222222222214</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="32">
         <f t="shared" si="0"/>
         <v>70.830398726074264</v>
       </c>
-      <c r="F18" s="41">
+      <c r="F18" s="40">
         <f t="shared" ref="F18:F24" si="6">F19+F$50</f>
         <v>1.350000000000003</v>
       </c>
-      <c r="G18" s="33">
+      <c r="G18" s="32">
         <f t="shared" si="1"/>
         <v>72.180398726074273</v>
       </c>
@@ -10868,15 +10928,15 @@
       <c r="C19" s="3">
         <v>71.111111111111114</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="32">
         <f t="shared" si="0"/>
         <v>69.724270705990051</v>
       </c>
-      <c r="F19" s="41">
+      <c r="F19" s="40">
         <f t="shared" si="6"/>
         <v>1.3650000000000029</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="32">
         <f t="shared" si="1"/>
         <v>71.08927070599006</v>
       </c>
@@ -10896,15 +10956,15 @@
       <c r="C20" s="3">
         <v>68.888888888888886</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="32">
         <f t="shared" si="0"/>
         <v>67.520601798136738</v>
       </c>
-      <c r="F20" s="41">
+      <c r="F20" s="40">
         <f t="shared" si="6"/>
         <v>1.3800000000000028</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="32">
         <f t="shared" si="1"/>
         <v>68.900601798136748</v>
       </c>
@@ -10924,15 +10984,15 @@
       <c r="C21" s="3">
         <v>66.666666666666671</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="32">
         <f t="shared" si="0"/>
         <v>65.371796767566536</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="40">
         <f t="shared" si="6"/>
         <v>1.3950000000000027</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G21" s="32">
         <f t="shared" si="1"/>
         <v>66.766796767566532</v>
       </c>
@@ -10952,15 +11012,15 @@
       <c r="C22" s="3">
         <v>65.555555555555557</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="32">
         <f t="shared" si="0"/>
         <v>64.156878707749783</v>
       </c>
-      <c r="F22" s="41">
+      <c r="F22" s="40">
         <f t="shared" si="6"/>
         <v>1.4100000000000026</v>
       </c>
-      <c r="G22" s="33">
+      <c r="G22" s="32">
         <f t="shared" si="1"/>
         <v>65.56687870774978</v>
       </c>
@@ -10980,15 +11040,15 @@
       <c r="C23" s="3">
         <v>64.444444444444443</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="32">
         <f t="shared" si="0"/>
         <v>63.08759969424446</v>
       </c>
-      <c r="F23" s="41">
+      <c r="F23" s="40">
         <f t="shared" si="6"/>
         <v>1.4250000000000025</v>
       </c>
-      <c r="G23" s="33">
+      <c r="G23" s="32">
         <f t="shared" si="1"/>
         <v>64.512599694244457</v>
       </c>
@@ -11008,15 +11068,15 @@
       <c r="C24" s="3">
         <v>62.777777777777779</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="32">
         <f t="shared" si="0"/>
         <v>61.332000755326007</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F24" s="40">
         <f t="shared" si="6"/>
         <v>1.4400000000000024</v>
       </c>
-      <c r="G24" s="33">
+      <c r="G24" s="32">
         <f t="shared" si="1"/>
         <v>62.772000755326012</v>
       </c>
@@ -11036,15 +11096,15 @@
       <c r="C25" s="3">
         <v>60</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="32">
         <f t="shared" si="0"/>
         <v>58.363483054889628</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F25" s="40">
         <f t="shared" ref="F25:F46" si="7">F26+F$50</f>
         <v>1.4550000000000023</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G25" s="32">
         <f t="shared" si="1"/>
         <v>59.818483054889633</v>
       </c>
@@ -11064,15 +11124,15 @@
       <c r="C26" s="3">
         <v>55.555555555555557</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="32">
         <f t="shared" si="0"/>
         <v>53.786784148048866</v>
       </c>
-      <c r="F26" s="41">
+      <c r="F26" s="40">
         <f t="shared" si="7"/>
         <v>1.4700000000000022</v>
       </c>
-      <c r="G26" s="33">
+      <c r="G26" s="32">
         <f t="shared" si="1"/>
         <v>55.256784148048865</v>
       </c>
@@ -11092,15 +11152,15 @@
       <c r="C27" s="3">
         <v>52.777777777777779</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="32">
         <f t="shared" si="0"/>
         <v>51.138705111395296</v>
       </c>
-      <c r="F27" s="41">
+      <c r="F27" s="40">
         <f t="shared" si="7"/>
         <v>1.4850000000000021</v>
       </c>
-      <c r="G27" s="33">
+      <c r="G27" s="32">
         <f t="shared" si="1"/>
         <v>52.623705111395296</v>
       </c>
@@ -11120,15 +11180,15 @@
       <c r="C28" s="3">
         <v>51.666666666666664</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="32">
         <f t="shared" si="0"/>
         <v>49.995767888660652</v>
       </c>
-      <c r="F28" s="41">
+      <c r="F28" s="40">
         <f t="shared" si="7"/>
         <v>1.500000000000002</v>
       </c>
-      <c r="G28" s="33">
+      <c r="G28" s="32">
         <f t="shared" si="1"/>
         <v>51.495767888660652</v>
       </c>
@@ -11148,15 +11208,15 @@
       <c r="C29" s="3">
         <v>50.555555555555557</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="32">
         <f t="shared" si="0"/>
         <v>48.900394114646886</v>
       </c>
-      <c r="F29" s="41">
+      <c r="F29" s="40">
         <f t="shared" si="7"/>
         <v>1.5150000000000019</v>
       </c>
-      <c r="G29" s="33">
+      <c r="G29" s="32">
         <f t="shared" si="1"/>
         <v>50.415394114646887</v>
       </c>
@@ -11176,15 +11236,15 @@
       <c r="C30" s="3">
         <v>50</v>
       </c>
-      <c r="E30" s="33">
+      <c r="E30" s="32">
         <f t="shared" si="0"/>
         <v>48.341761904105823</v>
       </c>
-      <c r="F30" s="41">
+      <c r="F30" s="40">
         <f t="shared" si="7"/>
         <v>1.5300000000000018</v>
       </c>
-      <c r="G30" s="33">
+      <c r="G30" s="32">
         <f t="shared" si="1"/>
         <v>49.871761904105824</v>
       </c>
@@ -11204,15 +11264,15 @@
       <c r="C31" s="3">
         <v>47.777777777777779</v>
       </c>
-      <c r="E31" s="33">
+      <c r="E31" s="32">
         <f t="shared" si="0"/>
         <v>45.966465564039211</v>
       </c>
-      <c r="F31" s="41">
+      <c r="F31" s="40">
         <f t="shared" si="7"/>
         <v>1.5450000000000017</v>
       </c>
-      <c r="G31" s="33">
+      <c r="G31" s="32">
         <f t="shared" si="1"/>
         <v>47.511465564039213</v>
       </c>
@@ -11232,15 +11292,15 @@
       <c r="C32" s="3">
         <v>46.666666666666664</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="32">
         <f t="shared" si="0"/>
         <v>44.928515443155298</v>
       </c>
-      <c r="F32" s="41">
+      <c r="F32" s="40">
         <f t="shared" si="7"/>
         <v>1.5600000000000016</v>
       </c>
-      <c r="G32" s="33">
+      <c r="G32" s="32">
         <f t="shared" si="1"/>
         <v>46.4885154431553</v>
       </c>
@@ -11260,15 +11320,15 @@
       <c r="C33" s="3">
         <v>45.555555555555557</v>
       </c>
-      <c r="E33" s="33">
+      <c r="E33" s="32">
         <f t="shared" si="0"/>
         <v>44.117971865634445</v>
       </c>
-      <c r="F33" s="41">
+      <c r="F33" s="40">
         <f t="shared" si="7"/>
         <v>1.5750000000000015</v>
       </c>
-      <c r="G33" s="33">
+      <c r="G33" s="32">
         <f t="shared" si="1"/>
         <v>45.692971865634448</v>
       </c>
@@ -11288,15 +11348,15 @@
       <c r="C34" s="3">
         <v>42.777777777777779</v>
       </c>
-      <c r="E34" s="33">
+      <c r="E34" s="32">
         <f t="shared" si="0"/>
         <v>41.659502454795899</v>
       </c>
-      <c r="F34" s="41">
+      <c r="F34" s="40">
         <f t="shared" si="7"/>
         <v>1.5900000000000014</v>
       </c>
-      <c r="G34" s="33">
+      <c r="G34" s="32">
         <f t="shared" si="1"/>
         <v>43.249502454795902</v>
       </c>
@@ -11316,15 +11376,15 @@
       <c r="C35" s="3">
         <v>40</v>
       </c>
-      <c r="E35" s="33">
+      <c r="E35" s="32">
         <f t="shared" si="0"/>
         <v>38.804048864842798</v>
       </c>
-      <c r="F35" s="41">
+      <c r="F35" s="40">
         <f t="shared" si="7"/>
         <v>1.6050000000000013</v>
       </c>
-      <c r="G35" s="33">
+      <c r="G35" s="32">
         <f t="shared" si="1"/>
         <v>40.409048864842802</v>
       </c>
@@ -11344,15 +11404,15 @@
       <c r="C36" s="3">
         <v>37.777777777777779</v>
       </c>
-      <c r="E36" s="33">
+      <c r="E36" s="32">
         <f t="shared" si="0"/>
         <v>36.449927486993147</v>
       </c>
-      <c r="F36" s="41">
+      <c r="F36" s="40">
         <f t="shared" si="7"/>
         <v>1.6200000000000012</v>
       </c>
-      <c r="G36" s="33">
+      <c r="G36" s="32">
         <f t="shared" si="1"/>
         <v>38.069927486993151</v>
       </c>
@@ -11372,15 +11432,15 @@
       <c r="C37" s="3">
         <v>36.666666666666664</v>
       </c>
-      <c r="E37" s="33">
+      <c r="E37" s="32">
         <f t="shared" si="0"/>
         <v>35.270131656675808</v>
       </c>
-      <c r="F37" s="41">
+      <c r="F37" s="40">
         <f t="shared" si="7"/>
         <v>1.6350000000000011</v>
       </c>
-      <c r="G37" s="33">
+      <c r="G37" s="32">
         <f t="shared" si="1"/>
         <v>36.905131656675806</v>
       </c>
@@ -11400,15 +11460,15 @@
       <c r="C38" s="3">
         <v>35.555555555555557</v>
       </c>
-      <c r="E38" s="33">
+      <c r="E38" s="32">
         <f t="shared" si="0"/>
         <v>34.082257595815797</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F38" s="40">
         <f t="shared" si="7"/>
         <v>1.650000000000001</v>
       </c>
-      <c r="G38" s="33">
+      <c r="G38" s="32">
         <f t="shared" si="1"/>
         <v>35.732257595815796</v>
       </c>
@@ -11428,15 +11488,15 @@
       <c r="C39" s="3">
         <v>33.888888888888886</v>
       </c>
-      <c r="E39" s="33">
+      <c r="E39" s="32">
         <f t="shared" si="0"/>
         <v>32.359778917868567</v>
       </c>
-      <c r="F39" s="41">
+      <c r="F39" s="40">
         <f t="shared" si="7"/>
         <v>1.6650000000000009</v>
       </c>
-      <c r="G39" s="33">
+      <c r="G39" s="32">
         <f t="shared" si="1"/>
         <v>34.024778917868566</v>
       </c>
@@ -11456,15 +11516,15 @@
       <c r="C40" s="3">
         <v>32.777777777777779</v>
       </c>
-      <c r="E40" s="33">
+      <c r="E40" s="32">
         <f t="shared" si="0"/>
         <v>31.165645239518565</v>
       </c>
-      <c r="F40" s="41">
+      <c r="F40" s="40">
         <f t="shared" si="7"/>
         <v>1.6800000000000008</v>
       </c>
-      <c r="G40" s="33">
+      <c r="G40" s="32">
         <f t="shared" si="1"/>
         <v>32.845645239518568</v>
       </c>
@@ -11484,15 +11544,15 @@
       <c r="C41" s="3">
         <v>31.666666666666664</v>
       </c>
-      <c r="E41" s="33">
+      <c r="E41" s="32">
         <f t="shared" si="0"/>
         <v>29.897120333647258</v>
       </c>
-      <c r="F41" s="41">
+      <c r="F41" s="40">
         <f t="shared" si="7"/>
         <v>1.6950000000000007</v>
       </c>
-      <c r="G41" s="33">
+      <c r="G41" s="32">
         <f t="shared" si="1"/>
         <v>31.592120333647259</v>
       </c>
@@ -11512,15 +11572,15 @@
       <c r="C42" s="3">
         <v>29.444444444444443</v>
       </c>
-      <c r="E42" s="33">
+      <c r="E42" s="32">
         <f t="shared" si="0"/>
         <v>27.69228033454543</v>
       </c>
-      <c r="F42" s="41">
+      <c r="F42" s="40">
         <f t="shared" si="7"/>
         <v>1.7100000000000006</v>
       </c>
-      <c r="G42" s="33">
+      <c r="G42" s="32">
         <f t="shared" si="1"/>
         <v>29.402280334545431</v>
       </c>
@@ -11540,15 +11600,15 @@
       <c r="C43" s="3">
         <v>28.333333333333332</v>
       </c>
-      <c r="E43" s="33">
+      <c r="E43" s="32">
         <f t="shared" si="0"/>
         <v>26.255961623520534</v>
       </c>
-      <c r="F43" s="41">
+      <c r="F43" s="40">
         <f t="shared" si="7"/>
         <v>1.7250000000000005</v>
       </c>
-      <c r="G43" s="33">
+      <c r="G43" s="32">
         <f t="shared" si="1"/>
         <v>27.980961623520535</v>
       </c>
@@ -11568,15 +11628,15 @@
       <c r="C44" s="3">
         <v>25.555555555555554</v>
       </c>
-      <c r="E44" s="33">
+      <c r="E44" s="32">
         <f t="shared" si="0"/>
         <v>23.449621292778104</v>
       </c>
-      <c r="F44" s="41">
+      <c r="F44" s="40">
         <f t="shared" si="7"/>
         <v>1.7400000000000004</v>
       </c>
-      <c r="G44" s="33">
+      <c r="G44" s="32">
         <f t="shared" si="1"/>
         <v>25.189621292778106</v>
       </c>
@@ -11596,15 +11656,15 @@
       <c r="C45" s="3">
         <v>23.333333333333332</v>
       </c>
-      <c r="E45" s="33">
+      <c r="E45" s="32">
         <f t="shared" si="0"/>
         <v>21.694857206695026</v>
       </c>
-      <c r="F45" s="41">
+      <c r="F45" s="40">
         <f t="shared" si="7"/>
         <v>1.7550000000000003</v>
       </c>
-      <c r="G45" s="33">
+      <c r="G45" s="32">
         <f>E45+F45</f>
         <v>23.449857206695025</v>
       </c>
@@ -11749,10 +11809,10 @@
     </row>
     <row r="51" spans="6:19" x14ac:dyDescent="0.25">
       <c r="L51" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="M51" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="Q51">
         <v>9</v>
@@ -11762,8 +11822,8 @@
       </c>
     </row>
     <row r="52" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="L52" s="31" t="s">
-        <v>97</v>
+      <c r="L52" s="30" t="s">
+        <v>92</v>
       </c>
       <c r="M52">
         <v>100</v>
@@ -11780,8 +11840,8 @@
       </c>
     </row>
     <row r="53" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="L53" s="31" t="s">
-        <v>93</v>
+      <c r="L53" s="30" t="s">
+        <v>88</v>
       </c>
       <c r="M53">
         <v>125</v>
@@ -11798,8 +11858,8 @@
       </c>
     </row>
     <row r="54" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="L54" s="31" t="s">
-        <v>94</v>
+      <c r="L54" s="30" t="s">
+        <v>89</v>
       </c>
       <c r="M54">
         <v>135</v>
@@ -11810,8 +11870,8 @@
       </c>
     </row>
     <row r="56" spans="6:19" x14ac:dyDescent="0.25">
-      <c r="L56" s="31" t="s">
-        <v>93</v>
+      <c r="L56" s="30" t="s">
+        <v>88</v>
       </c>
       <c r="M56">
         <v>135</v>
@@ -11864,18 +11924,18 @@
       <c r="B2">
         <v>6.8947599999999998E-2</v>
       </c>
-      <c r="G2" s="35">
+      <c r="G2" s="34">
         <v>-0.29666662644569519</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H2" s="31">
         <v>2.5286608389334247E-2</v>
       </c>
-      <c r="I2" s="36">
+      <c r="I2" s="35">
         <v>3.5048588958920229E-5</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="K3" s="34">
+      <c r="K3" s="33">
         <v>2E-3</v>
       </c>
     </row>
@@ -11887,7 +11947,7 @@
         <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
@@ -11916,7 +11976,7 @@
         <f>K5+E5</f>
         <v>-1.4273054898989151E-2</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M5" s="33">
         <f>(L5-C5)^2</f>
         <v>2.0372009614955819E-4</v>
       </c>
@@ -11948,7 +12008,7 @@
         <f t="shared" ref="L6:L33" si="3">K6+E6</f>
         <v>0.25180857746120783</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6" s="33">
         <f t="shared" ref="M6:M33" si="4">(L6-C6)^2</f>
         <v>5.7512781228211986E-4</v>
       </c>
@@ -11980,7 +12040,7 @@
         <f t="shared" si="3"/>
         <v>0.35870039808914772</v>
       </c>
-      <c r="M7" s="34">
+      <c r="M7" s="33">
         <f t="shared" si="4"/>
         <v>1.9494856039983623E-4</v>
       </c>
@@ -12012,7 +12072,7 @@
         <f t="shared" si="3"/>
         <v>0.54889005543395231</v>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="33">
         <f t="shared" si="4"/>
         <v>7.2401063197150958E-6</v>
       </c>
@@ -12044,7 +12104,7 @@
         <f t="shared" si="3"/>
         <v>0.7452173268227904</v>
       </c>
-      <c r="M9" s="34">
+      <c r="M9" s="33">
         <f t="shared" si="4"/>
         <v>1.7440565123108496E-4</v>
       </c>
@@ -12076,7 +12136,7 @@
         <f t="shared" si="3"/>
         <v>0.94497935992960269</v>
       </c>
-      <c r="M10" s="34">
+      <c r="M10" s="33">
         <f t="shared" si="4"/>
         <v>2.3678500926624579E-3</v>
       </c>
@@ -12108,7 +12168,7 @@
         <f t="shared" si="3"/>
         <v>1.0788074601066415</v>
       </c>
-      <c r="M11" s="34">
+      <c r="M11" s="33">
         <f t="shared" si="4"/>
         <v>1.988576684282632E-3</v>
       </c>
@@ -12140,7 +12200,7 @@
         <f t="shared" si="3"/>
         <v>1.2141188165684222</v>
       </c>
-      <c r="M12" s="34">
+      <c r="M12" s="33">
         <f t="shared" si="4"/>
         <v>1.7648078842258598E-3</v>
       </c>
@@ -12172,7 +12232,7 @@
         <f t="shared" si="3"/>
         <v>1.2862613840603827</v>
       </c>
-      <c r="M13" s="34">
+      <c r="M13" s="33">
         <f t="shared" si="4"/>
         <v>5.6373080590891883E-4</v>
       </c>
@@ -12204,7 +12264,7 @@
         <f t="shared" si="3"/>
         <v>1.4951500697320979</v>
       </c>
-      <c r="M14" s="34">
+      <c r="M14" s="33">
         <f t="shared" si="4"/>
         <v>4.7076546186231336E-4</v>
       </c>
@@ -12236,7 +12296,7 @@
         <f t="shared" si="3"/>
         <v>1.6349756844517871</v>
       </c>
-      <c r="M15" s="34">
+      <c r="M15" s="33">
         <f t="shared" si="4"/>
         <v>3.9072304356395978E-4</v>
       </c>
@@ -12268,7 +12328,7 @@
         <f t="shared" si="3"/>
         <v>1.9201538540015308</v>
       </c>
-      <c r="M16" s="34">
+      <c r="M16" s="33">
         <f t="shared" si="4"/>
         <v>1.0772252003913802E-4</v>
       </c>
@@ -12300,7 +12360,7 @@
         <f t="shared" si="3"/>
         <v>2.0644614822772871</v>
       </c>
-      <c r="M17" s="34">
+      <c r="M17" s="33">
         <f t="shared" si="4"/>
         <v>1.5733262844595027E-5</v>
       </c>
@@ -12332,7 +12392,7 @@
         <f t="shared" si="3"/>
         <v>2.2102523668377843</v>
       </c>
-      <c r="M18" s="34">
+      <c r="M18" s="33">
         <f t="shared" si="4"/>
         <v>4.2273966508695063E-3</v>
       </c>
@@ -12364,7 +12424,7 @@
         <f t="shared" si="3"/>
         <v>2.4339105278967885</v>
       </c>
-      <c r="M19" s="34">
+      <c r="M19" s="33">
         <f t="shared" si="4"/>
         <v>4.3033543766064048E-4</v>
       </c>
@@ -12396,7 +12456,7 @@
         <f t="shared" si="3"/>
         <v>2.5094907558482924</v>
       </c>
-      <c r="M20" s="34">
+      <c r="M20" s="33">
         <f t="shared" si="4"/>
         <v>7.4950866234169502E-4</v>
       </c>
@@ -12428,7 +12488,7 @@
         <f t="shared" si="3"/>
         <v>2.7344563241299173</v>
       </c>
-      <c r="M21" s="34">
+      <c r="M21" s="33">
         <f t="shared" si="4"/>
         <v>5.4979350370845204E-4</v>
       </c>
@@ -12460,7 +12520,7 @@
         <f t="shared" si="3"/>
         <v>2.8902422704352664</v>
       </c>
-      <c r="M22" s="34">
+      <c r="M22" s="33">
         <f t="shared" si="4"/>
         <v>3.0879466187409531E-5</v>
       </c>
@@ -12492,7 +12552,7 @@
         <f t="shared" si="3"/>
         <v>3.0442555539655269</v>
       </c>
-      <c r="M23" s="34">
+      <c r="M23" s="33">
         <f t="shared" si="4"/>
         <v>1.1153797308356746E-4</v>
       </c>
@@ -12524,7 +12584,7 @@
         <f t="shared" si="3"/>
         <v>3.2031054479176659</v>
       </c>
-      <c r="M24" s="34">
+      <c r="M24" s="33">
         <f t="shared" si="4"/>
         <v>9.9324866996945487E-4</v>
       </c>
@@ -12556,7 +12616,7 @@
         <f t="shared" si="3"/>
         <v>3.2487628401323496</v>
       </c>
-      <c r="M25" s="34">
+      <c r="M25" s="33">
         <f t="shared" si="4"/>
         <v>6.7661155586922335E-5</v>
       </c>
@@ -12588,7 +12648,7 @@
         <f t="shared" si="3"/>
         <v>3.4401797302268218</v>
       </c>
-      <c r="M26" s="34">
+      <c r="M26" s="33">
         <f t="shared" si="4"/>
         <v>5.1843884806542411E-5</v>
       </c>
@@ -12620,7 +12680,7 @@
         <f t="shared" si="3"/>
         <v>3.5994166554555194</v>
       </c>
-      <c r="M27" s="34">
+      <c r="M27" s="33">
         <f t="shared" si="4"/>
         <v>1.9998076240044168E-4</v>
       </c>
@@ -12652,7 +12712,7 @@
         <f t="shared" si="3"/>
         <v>3.6014166554555191</v>
       </c>
-      <c r="M28" s="34">
+      <c r="M28" s="33">
         <f t="shared" si="4"/>
         <v>2.605465842225125E-4</v>
       </c>
@@ -12684,7 +12744,7 @@
         <f t="shared" si="3"/>
         <v>3.6825913391766467</v>
       </c>
-      <c r="M29" s="34">
+      <c r="M29" s="33">
         <f t="shared" si="4"/>
         <v>1.6466601773053955E-3</v>
       </c>
@@ -12716,7 +12776,7 @@
         <f t="shared" si="3"/>
         <v>3.7641368369689592</v>
       </c>
-      <c r="M30" s="34">
+      <c r="M30" s="33">
         <f t="shared" si="4"/>
         <v>7.8294548456967882E-4</v>
       </c>
@@ -12748,7 +12808,7 @@
         <f t="shared" si="3"/>
         <v>3.9298394310343454</v>
       </c>
-      <c r="M31" s="34">
+      <c r="M31" s="33">
         <f t="shared" si="4"/>
         <v>3.0195653424622242E-8</v>
       </c>
@@ -12780,7 +12840,7 @@
         <f t="shared" si="3"/>
         <v>4.1749740603182701</v>
       </c>
-      <c r="M32" s="34">
+      <c r="M32" s="33">
         <f t="shared" si="4"/>
         <v>1.4529865224272892E-3</v>
       </c>
@@ -12812,7 +12872,7 @@
         <f t="shared" si="3"/>
         <v>4.2623249115312865</v>
       </c>
-      <c r="M33" s="34">
+      <c r="M33" s="33">
         <f t="shared" si="4"/>
         <v>1.5441264510767982E-4</v>
       </c>
@@ -12872,13 +12932,13 @@
         <v>17</v>
       </c>
       <c r="M39" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
-      <c r="K40" s="31" t="s">
-        <v>94</v>
+      <c r="K40" s="30" t="s">
+        <v>89</v>
       </c>
       <c r="L40">
         <v>6</v>
@@ -12890,8 +12950,8 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
-      <c r="K41" s="31" t="s">
-        <v>93</v>
+      <c r="K41" s="30" t="s">
+        <v>88</v>
       </c>
       <c r="L41" s="3">
         <v>5.5</v>
@@ -12903,8 +12963,8 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
-      <c r="K42" s="31" t="s">
-        <v>92</v>
+      <c r="K42" s="30" t="s">
+        <v>87</v>
       </c>
       <c r="L42">
         <v>1.3</v>
@@ -12916,8 +12976,8 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
-      <c r="K43" s="31" t="s">
-        <v>96</v>
+      <c r="K43" s="30" t="s">
+        <v>91</v>
       </c>
       <c r="L43">
         <v>0.8</v>
@@ -13018,12 +13078,12 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -13040,7 +13100,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -13057,7 +13117,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -13099,7 +13159,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C7">
         <f>(C3/1000)*C5</f>
@@ -13114,7 +13174,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C8">
         <f>(C4/1000)*C5</f>
@@ -13129,7 +13189,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C9">
         <f>C2-C8</f>
@@ -13144,7 +13204,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C10">
         <f>C2-C7</f>
@@ -13219,7 +13279,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C17">
         <v>50</v>
@@ -13233,7 +13293,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C18">
         <v>1000</v>
@@ -13247,7 +13307,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C19" s="3">
         <f>(C17-ROTOR_A)/ROTOR_B</f>
@@ -13256,7 +13316,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C20" s="3">
         <f>(C18-ROTOR_A)/ROTOR_B</f>
@@ -13265,18 +13325,18 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>160</v>
-      </c>
-      <c r="C21" s="34">
+        <v>153</v>
+      </c>
+      <c r="C21" s="33">
         <f>C19*$C$5/1000</f>
         <v>0.22559999999999999</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" s="34">
+        <v>156</v>
+      </c>
+      <c r="C22" s="33">
         <f>C20*$C$5/1000</f>
         <v>0.94</v>
       </c>
@@ -13321,10 +13381,10 @@
       <c r="B2" s="2">
         <v>-137.69868567406144</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="34">
         <v>9.5067552553605665</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>-0.27222557461004249</v>
       </c>
     </row>
@@ -13333,15 +13393,15 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="55">
+        <v>150</v>
+      </c>
+      <c r="F4" s="54">
         <f>SUM(F5:F252)</f>
         <v>27.870174821385483</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="54">
+      <c r="A5" s="53">
         <v>32205.9</v>
       </c>
       <c r="B5">
@@ -13357,7 +13417,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="54">
+      <c r="A6" s="53">
         <v>31074.799999999999</v>
       </c>
       <c r="B6">
@@ -13373,7 +13433,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="54">
+      <c r="A7" s="53">
         <v>29990</v>
       </c>
       <c r="B7">
@@ -13389,7 +13449,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="54">
+      <c r="A8" s="53">
         <v>28905.3</v>
       </c>
       <c r="B8">
@@ -13405,7 +13465,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="54">
+      <c r="A9" s="53">
         <v>27866</v>
       </c>
       <c r="B9">
@@ -13421,7 +13481,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="54">
+      <c r="A10" s="53">
         <v>26870</v>
       </c>
       <c r="B10">
@@ -13437,7 +13497,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="54">
+      <c r="A11" s="53">
         <v>25915.3</v>
       </c>
       <c r="B11">
@@ -13453,7 +13513,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="54">
+      <c r="A12" s="53">
         <v>25000</v>
       </c>
       <c r="B12">
@@ -13469,7 +13529,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="54">
+      <c r="A13" s="53">
         <v>24109.9</v>
       </c>
       <c r="B13">
@@ -13485,7 +13545,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="54">
+      <c r="A14" s="53">
         <v>23256.5</v>
       </c>
       <c r="B14">
@@ -13501,7 +13561,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="54">
+      <c r="A15" s="53">
         <v>22438.1</v>
       </c>
       <c r="B15">
@@ -13517,7 +13577,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="54">
+      <c r="A16" s="53">
         <v>21653.1</v>
       </c>
       <c r="B16">
@@ -13533,7 +13593,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="54">
+      <c r="A17" s="53">
         <v>20900</v>
       </c>
       <c r="B17">
@@ -13549,7 +13609,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="54">
+      <c r="A18" s="53">
         <v>20174.099999999999</v>
       </c>
       <c r="B18">
@@ -13565,7 +13625,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="54">
+      <c r="A19" s="53">
         <v>19477.399999999998</v>
       </c>
       <c r="B19">
@@ -13581,7 +13641,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="54">
+      <c r="A20" s="53">
         <v>18808.7</v>
       </c>
       <c r="B20">
@@ -13597,7 +13657,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="54">
+      <c r="A21" s="53">
         <v>18166.599999999999</v>
       </c>
       <c r="B21">
@@ -13613,7 +13673,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="54">
+      <c r="A22" s="53">
         <v>17550</v>
       </c>
       <c r="B22">
@@ -13629,7 +13689,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="54">
+      <c r="A23" s="53">
         <v>16945.900000000001</v>
       </c>
       <c r="B23">
@@ -13645,7 +13705,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="54">
+      <c r="A24" s="53">
         <v>16365.9</v>
       </c>
       <c r="B24">
@@ -13661,7 +13721,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="54">
+      <c r="A25" s="53">
         <v>15808.9</v>
       </c>
       <c r="B25">
@@ -13677,7 +13737,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="54">
+      <c r="A26" s="53">
         <v>15273.9</v>
       </c>
       <c r="B26">
@@ -13693,7 +13753,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="54">
+      <c r="A27" s="53">
         <v>14760</v>
       </c>
       <c r="B27">
@@ -13709,7 +13769,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="54">
+      <c r="A28" s="53">
         <v>14281.3</v>
       </c>
       <c r="B28">
@@ -13725,7 +13785,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="54">
+      <c r="A29" s="53">
         <v>13820.6</v>
       </c>
       <c r="B29">
@@ -13741,7 +13801,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="54">
+      <c r="A30" s="53">
         <v>13377.4</v>
       </c>
       <c r="B30">
@@ -13757,7 +13817,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="54">
+      <c r="A31" s="53">
         <v>12950.699999999999</v>
       </c>
       <c r="B31">
@@ -13773,7 +13833,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="54">
+      <c r="A32" s="53">
         <v>12540</v>
       </c>
       <c r="B32">
@@ -13789,7 +13849,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="54">
+      <c r="A33" s="53">
         <v>12134.7</v>
       </c>
       <c r="B33">
@@ -13805,7 +13865,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="54">
+      <c r="A34" s="53">
         <v>11744.7</v>
       </c>
       <c r="B34">
@@ -13821,7 +13881,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="54">
+      <c r="A35" s="53">
         <v>11369.400000000001</v>
       </c>
       <c r="B35">
@@ -13837,7 +13897,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="54">
+      <c r="A36" s="53">
         <v>11008</v>
       </c>
       <c r="B36">
@@ -13853,7 +13913,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="54">
+      <c r="A37" s="53">
         <v>10660</v>
       </c>
       <c r="B37">
@@ -13869,7 +13929,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="54">
+      <c r="A38" s="53">
         <v>10324.299999999999</v>
       </c>
       <c r="B38">
@@ -13885,7 +13945,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="54">
+      <c r="A39" s="53">
         <v>10001</v>
       </c>
       <c r="B39">
@@ -13901,7 +13961,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="54">
+      <c r="A40" s="53">
         <v>9689.5</v>
       </c>
       <c r="B40">
@@ -13917,7 +13977,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="54">
+      <c r="A41" s="53">
         <v>9389.3000000000011</v>
       </c>
       <c r="B41">
@@ -13933,7 +13993,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="54">
+      <c r="A42" s="53">
         <v>9100</v>
       </c>
       <c r="B42">
@@ -13949,7 +14009,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="54">
+      <c r="A43" s="53">
         <v>8817.1</v>
       </c>
       <c r="B43">
@@ -13965,7 +14025,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="54">
+      <c r="A44" s="53">
         <v>8544.4</v>
       </c>
       <c r="B44">
@@ -13981,7 +14041,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="54">
+      <c r="A45" s="53">
         <v>8281.5999999999985</v>
       </c>
       <c r="B45">
@@ -13997,7 +14057,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="54">
+      <c r="A46" s="53">
         <v>8028.3</v>
       </c>
       <c r="B46">
@@ -14013,7 +14073,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="54">
+      <c r="A47" s="53">
         <v>7784</v>
       </c>
       <c r="B47">
@@ -14029,7 +14089,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="54">
+      <c r="A48" s="53">
         <v>7553.8</v>
       </c>
       <c r="B48">
@@ -14045,7 +14105,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="54">
+      <c r="A49" s="53">
         <v>7331.5999999999995</v>
       </c>
       <c r="B49">
@@ -14061,7 +14121,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="54">
+      <c r="A50" s="53">
         <v>7117.2000000000007</v>
       </c>
       <c r="B50">
@@ -14077,7 +14137,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="54">
+      <c r="A51" s="53">
         <v>6910</v>
       </c>
       <c r="B51">
@@ -14093,7 +14153,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="54">
+      <c r="A52" s="53">
         <v>6710</v>
       </c>
       <c r="B52">
@@ -14109,7 +14169,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="54">
+      <c r="A53" s="53">
         <v>6526.5</v>
       </c>
       <c r="B53">
@@ -14125,7 +14185,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="54">
+      <c r="A54" s="53">
         <v>6349</v>
       </c>
       <c r="B54">
@@ -14141,7 +14201,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="54">
+      <c r="A55" s="53">
         <v>6177.2</v>
       </c>
       <c r="B55">
@@ -14157,7 +14217,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="54">
+      <c r="A56" s="53">
         <v>6010.9000000000005</v>
       </c>
       <c r="B56">
@@ -14173,7 +14233,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="54">
+      <c r="A57" s="53">
         <v>5850</v>
       </c>
       <c r="B57">
@@ -14189,7 +14249,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="54">
+      <c r="A58" s="53">
         <v>5683.2</v>
       </c>
       <c r="B58">
@@ -14205,7 +14265,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="54">
+      <c r="A59" s="53">
         <v>5522.1</v>
       </c>
       <c r="B59">
@@ -14221,7 +14281,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="54">
+      <c r="A60" s="53">
         <v>5366.3</v>
       </c>
       <c r="B60">
@@ -14237,7 +14297,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="54">
+      <c r="A61" s="53">
         <v>5215.6000000000004</v>
       </c>
       <c r="B61">
@@ -14253,7 +14313,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="54">
+      <c r="A62" s="53">
         <v>5070</v>
       </c>
       <c r="B62">
@@ -14269,7 +14329,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="54">
+      <c r="A63" s="53">
         <v>4929.1000000000004</v>
       </c>
       <c r="B63">
@@ -14285,7 +14345,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="54">
+      <c r="A64" s="53">
         <v>4792.7999999999993</v>
       </c>
       <c r="B64">
@@ -14301,7 +14361,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="54">
+      <c r="A65" s="53">
         <v>4661</v>
       </c>
       <c r="B65">
@@ -14317,7 +14377,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="54">
+      <c r="A66" s="53">
         <v>4533.4000000000005</v>
       </c>
       <c r="B66">
@@ -14333,7 +14393,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="54">
+      <c r="A67" s="53">
         <v>4410</v>
       </c>
       <c r="B67">
@@ -14349,7 +14409,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="54">
+      <c r="A68" s="53">
         <v>4290.6000000000004</v>
       </c>
       <c r="B68">
@@ -14365,7 +14425,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="54">
+      <c r="A69" s="53">
         <v>4175.0999999999995</v>
       </c>
       <c r="B69">
@@ -14381,7 +14441,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="54">
+      <c r="A70" s="53">
         <v>4063.2000000000003</v>
       </c>
       <c r="B70">
@@ -14397,7 +14457,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="54">
+      <c r="A71" s="53">
         <v>3954.8999999999996</v>
       </c>
       <c r="B71">
@@ -14413,7 +14473,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="54">
+      <c r="A72" s="53">
         <v>3850</v>
       </c>
       <c r="B72">
@@ -14429,7 +14489,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="54">
+      <c r="A73" s="53">
         <v>3741</v>
       </c>
       <c r="B73">
@@ -14445,7 +14505,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="54">
+      <c r="A74" s="53">
         <v>3635.7</v>
       </c>
       <c r="B74">
@@ -14461,7 +14521,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="54">
+      <c r="A75" s="53">
         <v>3533.7999999999997</v>
       </c>
       <c r="B75">
@@ -14477,7 +14537,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="54">
+      <c r="A76" s="53">
         <v>3435.2999999999997</v>
       </c>
       <c r="B76">
@@ -14493,7 +14553,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="54">
+      <c r="A77" s="53">
         <v>3340</v>
       </c>
       <c r="B77">
@@ -14509,7 +14569,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="54">
+      <c r="A78" s="53">
         <v>3255</v>
       </c>
       <c r="B78">
@@ -14525,7 +14585,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="54">
+      <c r="A79" s="53">
         <v>3172.6</v>
       </c>
       <c r="B79">
@@ -14541,7 +14601,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="54">
+      <c r="A80" s="53">
         <v>3092.7</v>
       </c>
       <c r="B80">
@@ -14557,7 +14617,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="54">
+      <c r="A81" s="53">
         <v>3015.2000000000003</v>
       </c>
       <c r="B81">
@@ -14573,7 +14633,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="54">
+      <c r="A82" s="53">
         <v>2940</v>
       </c>
       <c r="B82">
@@ -14589,7 +14649,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="54">
+      <c r="A83" s="53">
         <v>2863.4</v>
       </c>
       <c r="B83">
@@ -14605,7 +14665,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="54">
+      <c r="A84" s="53">
         <v>2789.2999999999997</v>
       </c>
       <c r="B84">
@@ -14621,7 +14681,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="54">
+      <c r="A85" s="53">
         <v>2717.2999999999997</v>
       </c>
       <c r="B85">
@@ -14637,7 +14697,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="54">
+      <c r="A86" s="53">
         <v>2647.6000000000004</v>
       </c>
       <c r="B86">
@@ -14653,7 +14713,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="54">
+      <c r="A87" s="53">
         <v>2580</v>
       </c>
       <c r="B87">
@@ -14669,7 +14729,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="54">
+      <c r="A88" s="53">
         <v>2514.4</v>
       </c>
       <c r="B88">
@@ -14685,7 +14745,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="54">
+      <c r="A89" s="53">
         <v>2450.6999999999998</v>
       </c>
       <c r="B89">
@@ -14701,7 +14761,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="54">
+      <c r="A90" s="53">
         <v>2389</v>
       </c>
       <c r="B90">
@@ -14717,7 +14777,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="54">
+      <c r="A91" s="53">
         <v>2329.1</v>
       </c>
       <c r="B91">
@@ -14733,7 +14793,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="54">
+      <c r="A92" s="53">
         <v>2271</v>
       </c>
       <c r="B92">
@@ -14749,7 +14809,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="54">
+      <c r="A93" s="53">
         <v>2213.5</v>
       </c>
       <c r="B93">
@@ -14765,7 +14825,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="54">
+      <c r="A94" s="53">
         <v>2157.7000000000003</v>
       </c>
       <c r="B94">
@@ -14781,7 +14841,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="54">
+      <c r="A95" s="53">
         <v>2103.5</v>
       </c>
       <c r="B95">
@@ -14797,7 +14857,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="54">
+      <c r="A96" s="53">
         <v>2051</v>
       </c>
       <c r="B96">
@@ -14813,7 +14873,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="54">
+      <c r="A97" s="53">
         <v>2000</v>
       </c>
       <c r="B97">
@@ -14829,7 +14889,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="54">
+      <c r="A98" s="53">
         <v>1951.3</v>
       </c>
       <c r="B98">
@@ -14845,7 +14905,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="54">
+      <c r="A99" s="53">
         <v>1904</v>
       </c>
       <c r="B99">
@@ -14861,7 +14921,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="54">
+      <c r="A100" s="53">
         <v>1858</v>
       </c>
       <c r="B100">
@@ -14877,7 +14937,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="54">
+      <c r="A101" s="53">
         <v>1813.3999999999999</v>
       </c>
       <c r="B101">
@@ -14893,7 +14953,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="54">
+      <c r="A102" s="53">
         <v>1770</v>
       </c>
       <c r="B102">
@@ -14909,7 +14969,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="54">
+      <c r="A103" s="53">
         <v>1731.9</v>
       </c>
       <c r="B103">
@@ -14925,7 +14985,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="54">
+      <c r="A104" s="53">
         <v>1694.7</v>
       </c>
       <c r="B104">
@@ -14941,7 +15001,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="54">
+      <c r="A105" s="53">
         <v>1658.6000000000001</v>
       </c>
       <c r="B105">
@@ -14957,7 +15017,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="54">
+      <c r="A106" s="53">
         <v>1623.3</v>
       </c>
       <c r="B106">
@@ -14973,7 +15033,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="54">
+      <c r="A107" s="53">
         <v>1589</v>
       </c>
       <c r="B107">
@@ -14989,7 +15049,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="54">
+      <c r="A108" s="53">
         <v>1552</v>
       </c>
       <c r="B108">
@@ -15005,7 +15065,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="54">
+      <c r="A109" s="53">
         <v>1516</v>
       </c>
       <c r="B109">
@@ -15021,7 +15081,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="54">
+      <c r="A110" s="53">
         <v>1481.1000000000001</v>
       </c>
       <c r="B110">
@@ -15037,7 +15097,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="54">
+      <c r="A111" s="53">
         <v>1447.1000000000001</v>
       </c>
       <c r="B111">
@@ -15053,7 +15113,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="54">
+      <c r="A112" s="53">
         <v>1414</v>
       </c>
       <c r="B112">
@@ -15069,7 +15129,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="54">
+      <c r="A113" s="53">
         <v>1381.2</v>
       </c>
       <c r="B113">
@@ -15085,7 +15145,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="54">
+      <c r="A114" s="53">
         <v>1349.3999999999999</v>
       </c>
       <c r="B114">
@@ -15101,7 +15161,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="54">
+      <c r="A115" s="53">
         <v>1318.4</v>
       </c>
       <c r="B115">
@@ -15117,7 +15177,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="54">
+      <c r="A116" s="53">
         <v>1288.3</v>
       </c>
       <c r="B116">
@@ -15133,7 +15193,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="54">
+      <c r="A117" s="53">
         <v>1259</v>
       </c>
       <c r="B117">
@@ -15149,7 +15209,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="54">
+      <c r="A118" s="53">
         <v>1230.0999999999999</v>
       </c>
       <c r="B118">
@@ -15165,7 +15225,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="54">
+      <c r="A119" s="53">
         <v>1201.8999999999999</v>
       </c>
       <c r="B119">
@@ -15181,7 +15241,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="54">
+      <c r="A120" s="53">
         <v>1174.5</v>
       </c>
       <c r="B120">
@@ -15197,7 +15257,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="54">
+      <c r="A121" s="53">
         <v>1147.8999999999999</v>
       </c>
       <c r="B121">
@@ -15213,7 +15273,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="54">
+      <c r="A122" s="53">
         <v>1122</v>
       </c>
       <c r="B122">
@@ -15229,7 +15289,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="54">
+      <c r="A123" s="53">
         <v>1095.5999999999999</v>
       </c>
       <c r="B123">
@@ -15245,7 +15305,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="54">
+      <c r="A124" s="53">
         <v>1069.9000000000001</v>
       </c>
       <c r="B124">
@@ -15261,7 +15321,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="54">
+      <c r="A125" s="53">
         <v>1044.8999999999999</v>
       </c>
       <c r="B125">
@@ -15277,7 +15337,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="54">
+      <c r="A126" s="53">
         <v>1020.5999999999999</v>
       </c>
       <c r="B126">
@@ -15293,7 +15353,7 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="54">
+      <c r="A127" s="53">
         <v>997</v>
       </c>
       <c r="B127">
@@ -15309,7 +15369,7 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="54">
+      <c r="A128" s="53">
         <v>975.7</v>
       </c>
       <c r="B128">
@@ -15325,7 +15385,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="54">
+      <c r="A129" s="53">
         <v>955</v>
       </c>
       <c r="B129">
@@ -15341,7 +15401,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="54">
+      <c r="A130" s="53">
         <v>934.8</v>
       </c>
       <c r="B130">
@@ -15357,7 +15417,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="54">
+      <c r="A131" s="53">
         <v>915.1</v>
       </c>
       <c r="B131">
@@ -15373,7 +15433,7 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="54">
+      <c r="A132" s="53">
         <v>896</v>
       </c>
       <c r="B132">
@@ -15389,7 +15449,7 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="54">
+      <c r="A133" s="53">
         <v>875</v>
       </c>
       <c r="B133">
@@ -15405,7 +15465,7 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="54">
+      <c r="A134" s="53">
         <v>854.7</v>
       </c>
       <c r="B134">
@@ -15421,7 +15481,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="54">
+      <c r="A135" s="53">
         <v>834.9</v>
       </c>
       <c r="B135">
@@ -15437,7 +15497,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="54">
+      <c r="A136" s="53">
         <v>815.69999999999993</v>
       </c>
       <c r="B136">
@@ -15453,7 +15513,7 @@
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="54">
+      <c r="A137" s="53">
         <v>797</v>
       </c>
       <c r="B137">
@@ -15469,7 +15529,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="54">
+      <c r="A138" s="53">
         <v>780.59999999999991</v>
       </c>
       <c r="B138">
@@ -15485,7 +15545,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" s="54">
+      <c r="A139" s="53">
         <v>764.59999999999991</v>
       </c>
       <c r="B139">
@@ -15501,7 +15561,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="54">
+      <c r="A140" s="53">
         <v>749</v>
       </c>
       <c r="B140">
@@ -15517,7 +15577,7 @@
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" s="54">
+      <c r="A141" s="53">
         <v>733.8</v>
       </c>
       <c r="B141">
@@ -15533,7 +15593,7 @@
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="54">
+      <c r="A142" s="53">
         <v>719</v>
       </c>
       <c r="B142">
@@ -15549,7 +15609,7 @@
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="54">
+      <c r="A143" s="53">
         <v>702.9</v>
       </c>
       <c r="B143">
@@ -15565,7 +15625,7 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="54">
+      <c r="A144" s="53">
         <v>687.30000000000007</v>
       </c>
       <c r="B144">
@@ -15581,7 +15641,7 @@
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="54">
+      <c r="A145" s="53">
         <v>672.1</v>
       </c>
       <c r="B145">
@@ -15597,7 +15657,7 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="54">
+      <c r="A146" s="53">
         <v>657.4</v>
       </c>
       <c r="B146">
@@ -15613,7 +15673,7 @@
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="54">
+      <c r="A147" s="53">
         <v>643</v>
       </c>
       <c r="B147">
@@ -15629,7 +15689,7 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="54">
+      <c r="A148" s="53">
         <v>630.19999999999993</v>
       </c>
       <c r="B148">
@@ -15645,7 +15705,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="54">
+      <c r="A149" s="53">
         <v>617.70000000000005</v>
       </c>
       <c r="B149">
@@ -15661,7 +15721,7 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="54">
+      <c r="A150" s="53">
         <v>605.5</v>
       </c>
       <c r="B150">
@@ -15677,7 +15737,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="54">
+      <c r="A151" s="53">
         <v>593.6</v>
       </c>
       <c r="B151">
@@ -15693,7 +15753,7 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="54">
+      <c r="A152" s="53">
         <v>582</v>
       </c>
       <c r="B152">
@@ -15709,7 +15769,7 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="54">
+      <c r="A153" s="53">
         <v>571.69999999999993</v>
       </c>
       <c r="B153">
@@ -15725,7 +15785,7 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" s="54">
+      <c r="A154" s="53">
         <v>561.69999999999993</v>
       </c>
       <c r="B154">
@@ -15741,7 +15801,7 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="54">
+      <c r="A155" s="53">
         <v>551.9</v>
       </c>
       <c r="B155">
@@ -15757,7 +15817,7 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="54">
+      <c r="A156" s="53">
         <v>542.29999999999995</v>
       </c>
       <c r="B156">
@@ -15773,7 +15833,7 @@
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" s="54">
+      <c r="A157" s="53">
         <v>533</v>
       </c>
       <c r="B157">
@@ -15789,7 +15849,7 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="54">
+      <c r="A158" s="53">
         <v>522.5</v>
       </c>
       <c r="B158">
@@ -15805,7 +15865,7 @@
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" s="54">
+      <c r="A159" s="53">
         <v>512.20000000000005</v>
       </c>
       <c r="B159">
@@ -15821,7 +15881,7 @@
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="54">
+      <c r="A160" s="53">
         <v>502.2</v>
       </c>
       <c r="B160">
@@ -15837,7 +15897,7 @@
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" s="54">
+      <c r="A161" s="53">
         <v>492.5</v>
       </c>
       <c r="B161">
@@ -15853,7 +15913,7 @@
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="54">
+      <c r="A162" s="53">
         <v>483</v>
       </c>
       <c r="B162">
@@ -15869,7 +15929,7 @@
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="54">
+      <c r="A163" s="53">
         <v>473.3</v>
       </c>
       <c r="B163">
@@ -15885,7 +15945,7 @@
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="54">
+      <c r="A164" s="53">
         <v>463.9</v>
       </c>
       <c r="B164">
@@ -15901,7 +15961,7 @@
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="54">
+      <c r="A165" s="53">
         <v>454.7</v>
       </c>
       <c r="B165">
@@ -15917,7 +15977,7 @@
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="54">
+      <c r="A166" s="53">
         <v>445.7</v>
       </c>
       <c r="B166">
@@ -15933,7 +15993,7 @@
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" s="54">
+      <c r="A167" s="53">
         <v>437</v>
       </c>
       <c r="B167">
@@ -15949,7 +16009,7 @@
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" s="54">
+      <c r="A168" s="53">
         <v>428.4</v>
       </c>
       <c r="B168">
@@ -15965,7 +16025,7 @@
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" s="54">
+      <c r="A169" s="53">
         <v>420</v>
       </c>
       <c r="B169">
@@ -15981,7 +16041,7 @@
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" s="54">
+      <c r="A170" s="53">
         <v>411.8</v>
       </c>
       <c r="B170">
@@ -15997,7 +16057,7 @@
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" s="54">
+      <c r="A171" s="53">
         <v>403.8</v>
       </c>
       <c r="B171">
@@ -16013,7 +16073,7 @@
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" s="54">
+      <c r="A172" s="53">
         <v>396</v>
       </c>
       <c r="B172">
@@ -16029,7 +16089,7 @@
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" s="54">
+      <c r="A173" s="53">
         <v>388.40000000000003</v>
       </c>
       <c r="B173">
@@ -16045,7 +16105,7 @@
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" s="54">
+      <c r="A174" s="53">
         <v>381</v>
       </c>
       <c r="B174">
@@ -16061,7 +16121,7 @@
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" s="54">
+      <c r="A175" s="53">
         <v>373.90000000000003</v>
       </c>
       <c r="B175">
@@ -16077,7 +16137,7 @@
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" s="54">
+      <c r="A176" s="53">
         <v>366.8</v>
       </c>
       <c r="B176">
@@ -16093,7 +16153,7 @@
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" s="54">
+      <c r="A177" s="53">
         <v>360</v>
       </c>
       <c r="B177">
@@ -16109,7 +16169,7 @@
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" s="54">
+      <c r="A178" s="53">
         <v>353.3</v>
       </c>
       <c r="B178">
@@ -16125,7 +16185,7 @@
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" s="54">
+      <c r="A179" s="53">
         <v>346.7</v>
       </c>
       <c r="B179">
@@ -16141,7 +16201,7 @@
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" s="54">
+      <c r="A180" s="53">
         <v>340.3</v>
       </c>
       <c r="B180">
@@ -16157,7 +16217,7 @@
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="54">
+      <c r="A181" s="53">
         <v>334.1</v>
       </c>
       <c r="B181">
@@ -16173,7 +16233,7 @@
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A182" s="54">
+      <c r="A182" s="53">
         <v>328</v>
       </c>
       <c r="B182">
@@ -16189,7 +16249,7 @@
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A183" s="54">
+      <c r="A183" s="53">
         <v>322</v>
       </c>
       <c r="B183">
@@ -16205,7 +16265,7 @@
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" s="54">
+      <c r="A184" s="53">
         <v>316.09999999999997</v>
       </c>
       <c r="B184">
@@ -16221,7 +16281,7 @@
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A185" s="54">
+      <c r="A185" s="53">
         <v>310.40000000000003</v>
       </c>
       <c r="B185">
@@ -16237,7 +16297,7 @@
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="54">
+      <c r="A186" s="53">
         <v>304.8</v>
       </c>
       <c r="B186">
@@ -16253,7 +16313,7 @@
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187" s="54">
+      <c r="A187" s="53">
         <v>299.3</v>
       </c>
       <c r="B187">
@@ -16269,7 +16329,7 @@
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A188" s="54">
+      <c r="A188" s="53">
         <v>294</v>
       </c>
       <c r="B188">
@@ -16285,7 +16345,7 @@
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="54">
+      <c r="A189" s="53">
         <v>288.8</v>
       </c>
       <c r="B189">
@@ -16301,7 +16361,7 @@
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="54">
+      <c r="A190" s="53">
         <v>283.60000000000002</v>
       </c>
       <c r="B190">
@@ -16317,7 +16377,7 @@
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="54">
+      <c r="A191" s="53">
         <v>278.60000000000002</v>
       </c>
       <c r="B191">
@@ -16333,7 +16393,7 @@
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A192" s="54">
+      <c r="A192" s="53">
         <v>273.7</v>
       </c>
       <c r="B192">
@@ -16349,7 +16409,7 @@
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A193" s="54">
+      <c r="A193" s="53">
         <v>268.89999999999998</v>
       </c>
       <c r="B193">
@@ -16365,7 +16425,7 @@
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" s="54">
+      <c r="A194" s="53">
         <v>264.2</v>
       </c>
       <c r="B194">
@@ -16381,7 +16441,7 @@
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A195" s="54">
+      <c r="A195" s="53">
         <v>259.60000000000002</v>
       </c>
       <c r="B195">
@@ -16397,7 +16457,7 @@
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="54">
+      <c r="A196" s="53">
         <v>255.1</v>
       </c>
       <c r="B196">
@@ -16413,7 +16473,7 @@
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="54">
+      <c r="A197" s="53">
         <v>250.7</v>
       </c>
       <c r="B197">
@@ -16429,7 +16489,7 @@
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" s="54">
+      <c r="A198" s="53">
         <v>246.4</v>
       </c>
       <c r="B198">
@@ -16445,7 +16505,7 @@
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="54">
+      <c r="A199" s="53">
         <v>242.2</v>
       </c>
       <c r="B199">
@@ -16461,7 +16521,7 @@
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" s="54">
+      <c r="A200" s="53">
         <v>238</v>
       </c>
       <c r="B200">
@@ -16477,7 +16537,7 @@
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" s="54">
+      <c r="A201" s="53">
         <v>234</v>
       </c>
       <c r="B201">
@@ -16493,7 +16553,7 @@
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A202" s="54">
+      <c r="A202" s="53">
         <v>230</v>
       </c>
       <c r="B202">
@@ -16509,7 +16569,7 @@
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A203" s="54">
+      <c r="A203" s="53">
         <v>226.20000000000002</v>
       </c>
       <c r="B203">
@@ -16525,7 +16585,7 @@
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" s="54">
+      <c r="A204" s="53">
         <v>222.3</v>
       </c>
       <c r="B204">
@@ -16541,7 +16601,7 @@
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A205" s="54">
+      <c r="A205" s="53">
         <v>218.6</v>
       </c>
       <c r="B205">
@@ -16557,7 +16617,7 @@
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" s="54">
+      <c r="A206" s="53">
         <v>215</v>
       </c>
       <c r="B206">
@@ -16573,7 +16633,7 @@
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A207" s="54">
+      <c r="A207" s="53">
         <v>211.4</v>
       </c>
       <c r="B207">
@@ -16589,7 +16649,7 @@
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A208" s="54">
+      <c r="A208" s="53">
         <v>207.9</v>
       </c>
       <c r="B208">
@@ -16605,7 +16665,7 @@
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A209" s="54">
+      <c r="A209" s="53">
         <v>204.5</v>
       </c>
       <c r="B209">
@@ -16621,7 +16681,7 @@
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210" s="54">
+      <c r="A210" s="53">
         <v>201.1</v>
       </c>
       <c r="B210">
@@ -16637,7 +16697,7 @@
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211" s="54">
+      <c r="A211" s="53">
         <v>197.8</v>
       </c>
       <c r="B211">
@@ -16653,7 +16713,7 @@
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" s="54">
+      <c r="A212" s="53">
         <v>194.6</v>
       </c>
       <c r="B212">
@@ -16669,7 +16729,7 @@
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="54">
+      <c r="A213" s="53">
         <v>191.39999999999998</v>
       </c>
       <c r="B213">
@@ -16685,7 +16745,7 @@
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="54">
+      <c r="A214" s="53">
         <v>188.29999999999998</v>
       </c>
       <c r="B214">
@@ -16701,7 +16761,7 @@
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="54">
+      <c r="A215" s="53">
         <v>185.29999999999998</v>
       </c>
       <c r="B215">
@@ -16717,7 +16777,7 @@
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="54">
+      <c r="A216" s="53">
         <v>182.29999999999998</v>
       </c>
       <c r="B216">
@@ -16733,7 +16793,7 @@
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="54">
+      <c r="A217" s="53">
         <v>179.4</v>
       </c>
       <c r="B217">
@@ -16749,7 +16809,7 @@
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="54">
+      <c r="A218" s="53">
         <v>176.5</v>
       </c>
       <c r="B218">
@@ -16765,7 +16825,7 @@
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="54">
+      <c r="A219" s="53">
         <v>173.7</v>
       </c>
       <c r="B219">
@@ -16781,7 +16841,7 @@
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="54">
+      <c r="A220" s="53">
         <v>171</v>
       </c>
       <c r="B220">
@@ -16797,7 +16857,7 @@
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="54">
+      <c r="A221" s="53">
         <v>168.3</v>
       </c>
       <c r="B221">
@@ -16813,7 +16873,7 @@
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" s="54">
+      <c r="A222" s="53">
         <v>165.6</v>
       </c>
       <c r="B222">
@@ -16829,7 +16889,7 @@
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="54">
+      <c r="A223" s="53">
         <v>163</v>
       </c>
       <c r="B223">
@@ -16845,7 +16905,7 @@
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="54">
+      <c r="A224" s="53">
         <v>160.39999999999998</v>
       </c>
       <c r="B224">
@@ -16861,7 +16921,7 @@
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A225" s="54">
+      <c r="A225" s="53">
         <v>157.9</v>
       </c>
       <c r="B225">
@@ -16877,7 +16937,7 @@
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="54">
+      <c r="A226" s="53">
         <v>155.5</v>
       </c>
       <c r="B226">
@@ -16893,7 +16953,7 @@
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" s="54">
+      <c r="A227" s="53">
         <v>153.10000000000002</v>
       </c>
       <c r="B227">
@@ -16909,7 +16969,7 @@
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A228" s="54">
+      <c r="A228" s="53">
         <v>150.69999999999999</v>
       </c>
       <c r="B228">
@@ -16925,7 +16985,7 @@
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A229" s="54">
+      <c r="A229" s="53">
         <v>148.4</v>
       </c>
       <c r="B229">
@@ -16941,7 +17001,7 @@
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" s="54">
+      <c r="A230" s="53">
         <v>146.1</v>
       </c>
       <c r="B230">
@@ -16957,7 +17017,7 @@
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="54">
+      <c r="A231" s="53">
         <v>143.9</v>
       </c>
       <c r="B231">
@@ -16973,7 +17033,7 @@
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="54">
+      <c r="A232" s="53">
         <v>141.69999999999999</v>
       </c>
       <c r="B232">
@@ -16989,7 +17049,7 @@
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="54">
+      <c r="A233" s="53">
         <v>139.6</v>
       </c>
       <c r="B233">
@@ -17005,7 +17065,7 @@
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="54">
+      <c r="A234" s="53">
         <v>137.5</v>
       </c>
       <c r="B234">
@@ -17021,7 +17081,7 @@
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A235" s="54">
+      <c r="A235" s="53">
         <v>135.4</v>
       </c>
       <c r="B235">
@@ -17037,7 +17097,7 @@
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="54">
+      <c r="A236" s="53">
         <v>133.39999999999998</v>
       </c>
       <c r="B236">
@@ -17053,7 +17113,7 @@
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A237" s="54">
+      <c r="A237" s="53">
         <v>131.39999999999998</v>
       </c>
       <c r="B237">
@@ -17069,7 +17129,7 @@
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A238" s="54">
+      <c r="A238" s="53">
         <v>129.5</v>
       </c>
       <c r="B238">
@@ -17085,7 +17145,7 @@
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A239" s="54">
+      <c r="A239" s="53">
         <v>127.5</v>
       </c>
       <c r="B239">
@@ -17101,7 +17161,7 @@
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A240" s="54">
+      <c r="A240" s="53">
         <v>125.7</v>
       </c>
       <c r="B240">
@@ -17117,7 +17177,7 @@
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="54">
+      <c r="A241" s="53">
         <v>123.8</v>
       </c>
       <c r="B241">
@@ -17133,7 +17193,7 @@
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" s="54">
+      <c r="A242" s="53">
         <v>122</v>
       </c>
       <c r="B242">
@@ -17149,7 +17209,7 @@
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A243" s="54">
+      <c r="A243" s="53">
         <v>120.2</v>
       </c>
       <c r="B243">
@@ -17165,7 +17225,7 @@
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" s="54">
+      <c r="A244" s="53">
         <v>118.5</v>
       </c>
       <c r="B244">
@@ -17181,7 +17241,7 @@
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A245" s="54">
+      <c r="A245" s="53">
         <v>116.8</v>
       </c>
       <c r="B245">
@@ -17197,7 +17257,7 @@
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A246" s="54">
+      <c r="A246" s="53">
         <v>115.1</v>
       </c>
       <c r="B246">
@@ -17213,7 +17273,7 @@
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A247" s="54">
+      <c r="A247" s="53">
         <v>113.4</v>
       </c>
       <c r="B247">
@@ -17229,7 +17289,7 @@
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A248" s="54">
+      <c r="A248" s="53">
         <v>111.8</v>
       </c>
       <c r="B248">
@@ -17245,7 +17305,7 @@
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A249" s="54">
+      <c r="A249" s="53">
         <v>110.2</v>
       </c>
       <c r="B249">
@@ -17261,7 +17321,7 @@
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" s="54">
+      <c r="A250" s="53">
         <v>108.60000000000001</v>
       </c>
       <c r="B250">
@@ -17277,7 +17337,7 @@
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" s="54">
+      <c r="A251" s="53">
         <v>107.1</v>
       </c>
       <c r="B251">
@@ -17293,7 +17353,7 @@
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A252" s="54">
+      <c r="A252" s="53">
         <v>105.6</v>
       </c>
       <c r="B252">

</xml_diff>